<commit_message>
Add oceania birds to translation tables
</commit_message>
<xml_diff>
--- a/i18n/de.xlsx
+++ b/i18n/de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matej\Programming\wingsearch\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej\Programming\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F909226F-58FF-41F0-B9BF-2E992BEEC828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AA659A-B4F0-45E8-9ED2-A42034AA28FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Birds!$A$1:$F$262</definedName>
-    <definedName name="ExternalData_2" localSheetId="1" hidden="1">Bonuses!$A$1:$G$34</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Birds!$A$1:$F$357</definedName>
+    <definedName name="ExternalData_2" localSheetId="1" hidden="1">Bonuses!$A$1:$G$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="1028">
   <si>
     <t>id</t>
   </si>
@@ -2541,6 +2541,591 @@
   </si>
   <si>
     <t>Goldammer</t>
+  </si>
+  <si>
+    <t>Abbott's Booby</t>
+  </si>
+  <si>
+    <t>Papasula abbotti</t>
+  </si>
+  <si>
+    <t>Australasian Pipit</t>
+  </si>
+  <si>
+    <t>Anthus novaeseelandiae</t>
+  </si>
+  <si>
+    <t>Australasian Shoveler</t>
+  </si>
+  <si>
+    <t>Spatula rhynchotis</t>
+  </si>
+  <si>
+    <t>Australian Ibis</t>
+  </si>
+  <si>
+    <t>Threskiornis moluccus</t>
+  </si>
+  <si>
+    <t>Australian Magpie</t>
+  </si>
+  <si>
+    <t>Gymnorhina tibicen</t>
+  </si>
+  <si>
+    <t>Australian Owlet-Nightjar</t>
+  </si>
+  <si>
+    <t>Aegotheles cristatus</t>
+  </si>
+  <si>
+    <t>Australian Raven</t>
+  </si>
+  <si>
+    <t>Corvus coronoides</t>
+  </si>
+  <si>
+    <t>Australian Reed Warbler</t>
+  </si>
+  <si>
+    <t>Acrocephalus australis</t>
+  </si>
+  <si>
+    <t>Australian Shelduck</t>
+  </si>
+  <si>
+    <t>Tadorna tadornoides</t>
+  </si>
+  <si>
+    <t>Australian Zebra Finch</t>
+  </si>
+  <si>
+    <t>Taeniopygia castanotis</t>
+  </si>
+  <si>
+    <t>Black Noddy</t>
+  </si>
+  <si>
+    <t>Anous minutus</t>
+  </si>
+  <si>
+    <t>Black Swan</t>
+  </si>
+  <si>
+    <t>Cygnus atratus</t>
+  </si>
+  <si>
+    <t>Black-Shouldered Kite</t>
+  </si>
+  <si>
+    <t>Elanus axillaris</t>
+  </si>
+  <si>
+    <t>Blyth's Hornbill</t>
+  </si>
+  <si>
+    <t>Rhyticeros plicatus</t>
+  </si>
+  <si>
+    <t>Brolga</t>
+  </si>
+  <si>
+    <t>Antigone rubicunda</t>
+  </si>
+  <si>
+    <t>Brown Falcon</t>
+  </si>
+  <si>
+    <t>Falco berigora</t>
+  </si>
+  <si>
+    <t>Budgerigar</t>
+  </si>
+  <si>
+    <t>Melopsittacus undulatus</t>
+  </si>
+  <si>
+    <t>Cockatiel</t>
+  </si>
+  <si>
+    <t>Nymphicus hollandicus</t>
+  </si>
+  <si>
+    <t>Count Raggi's Bird-of-Paradise</t>
+  </si>
+  <si>
+    <t>Paradisaea raggiana</t>
+  </si>
+  <si>
+    <t>Crested Pigeon</t>
+  </si>
+  <si>
+    <t>Ocyphaps lophotes</t>
+  </si>
+  <si>
+    <t>Crimson Chat</t>
+  </si>
+  <si>
+    <t>Epthianura tricolor</t>
+  </si>
+  <si>
+    <t>Eastern Rosella</t>
+  </si>
+  <si>
+    <t>Platycercus eximius</t>
+  </si>
+  <si>
+    <t>Eastern Whipbird</t>
+  </si>
+  <si>
+    <t>Psophodes olivaceus</t>
+  </si>
+  <si>
+    <t>Emu</t>
+  </si>
+  <si>
+    <t>Dromaius novaehollandiae</t>
+  </si>
+  <si>
+    <t>Galah</t>
+  </si>
+  <si>
+    <t>Eolophus roseicapilla</t>
+  </si>
+  <si>
+    <t>Golden-Headed Cisticola</t>
+  </si>
+  <si>
+    <t>Cisticola exilis</t>
+  </si>
+  <si>
+    <t>Gould's Finch</t>
+  </si>
+  <si>
+    <t>Erythrura gouldiae</t>
+  </si>
+  <si>
+    <t>Green Pygmy-Goose</t>
+  </si>
+  <si>
+    <t>Nettapus pulchellus</t>
+  </si>
+  <si>
+    <t>Grey Butcherbird</t>
+  </si>
+  <si>
+    <t>Cracticus torquatus</t>
+  </si>
+  <si>
+    <t>Grey Shrikethrush</t>
+  </si>
+  <si>
+    <t>Colluricincla harmonica</t>
+  </si>
+  <si>
+    <t>Grey Teal</t>
+  </si>
+  <si>
+    <t>Anas gracilis</t>
+  </si>
+  <si>
+    <t>Grey Warbler</t>
+  </si>
+  <si>
+    <t>Gerygone igata</t>
+  </si>
+  <si>
+    <t>Grey-Headed Mannikin</t>
+  </si>
+  <si>
+    <t>Lonchura caniceps</t>
+  </si>
+  <si>
+    <t>Horsfield's Bronze-Cuckoo</t>
+  </si>
+  <si>
+    <t>Chrysococcyx basalis</t>
+  </si>
+  <si>
+    <t>Horsfield's Bushlark</t>
+  </si>
+  <si>
+    <t>Mirafra javanica</t>
+  </si>
+  <si>
+    <t>Kākāpо̄</t>
+  </si>
+  <si>
+    <t>Strigops habroptila</t>
+  </si>
+  <si>
+    <t>Kea</t>
+  </si>
+  <si>
+    <t>Nestor notabilis</t>
+  </si>
+  <si>
+    <t>Kelp Gull</t>
+  </si>
+  <si>
+    <t>Larus dominicanus</t>
+  </si>
+  <si>
+    <t>Kererū</t>
+  </si>
+  <si>
+    <t>Hemiphaga novaeseelandiae</t>
+  </si>
+  <si>
+    <t>Korimako</t>
+  </si>
+  <si>
+    <t>Anthornis melanura</t>
+  </si>
+  <si>
+    <t>Laughing Kookaburra</t>
+  </si>
+  <si>
+    <t>Dacelo novaeguineae</t>
+  </si>
+  <si>
+    <t>Lesser Frigatebird</t>
+  </si>
+  <si>
+    <t>Fregata ariel</t>
+  </si>
+  <si>
+    <t>Lewin's Honeyeater</t>
+  </si>
+  <si>
+    <t>Meliphaga lewinii</t>
+  </si>
+  <si>
+    <t>Little Penguin</t>
+  </si>
+  <si>
+    <t>Eudyptula minor</t>
+  </si>
+  <si>
+    <t>Little Pied Cormorant</t>
+  </si>
+  <si>
+    <t>Microcarbo melanoleucos</t>
+  </si>
+  <si>
+    <t>Magpie-Lark</t>
+  </si>
+  <si>
+    <t>Grallina cyanoleuca</t>
+  </si>
+  <si>
+    <t>Major Mitchell's Cockatoo</t>
+  </si>
+  <si>
+    <t>Lophochroa leadbeateri</t>
+  </si>
+  <si>
+    <t>Malleefowl</t>
+  </si>
+  <si>
+    <t>Leipoa ocellata</t>
+  </si>
+  <si>
+    <t>Maned Duck</t>
+  </si>
+  <si>
+    <t>Chenonetta jubata</t>
+  </si>
+  <si>
+    <t>Many-Colored Fruit Dove</t>
+  </si>
+  <si>
+    <t>Ptilinopus perousii</t>
+  </si>
+  <si>
+    <t>Masked Lapwing</t>
+  </si>
+  <si>
+    <t>Vanellus miles</t>
+  </si>
+  <si>
+    <t>Mistletoebird</t>
+  </si>
+  <si>
+    <t>Dicaeum hirundinaceum</t>
+  </si>
+  <si>
+    <t>Musk Duck</t>
+  </si>
+  <si>
+    <t>Biziura lobata</t>
+  </si>
+  <si>
+    <t>New Holland Honeyeater</t>
+  </si>
+  <si>
+    <t>Phylidonyris novaehollandiae</t>
+  </si>
+  <si>
+    <t>Noisy Miner</t>
+  </si>
+  <si>
+    <t>Manorina melanocephala</t>
+  </si>
+  <si>
+    <t>North Island Brown Kiwi</t>
+  </si>
+  <si>
+    <t>Apteryx mantelli</t>
+  </si>
+  <si>
+    <t>Orange-Footed Scrubfowl</t>
+  </si>
+  <si>
+    <t>Megapodius reinwardt</t>
+  </si>
+  <si>
+    <t>Pacific Black Duck</t>
+  </si>
+  <si>
+    <t>Anas superciliosa</t>
+  </si>
+  <si>
+    <t>Peaceful Dove</t>
+  </si>
+  <si>
+    <t>Geopelia placida</t>
+  </si>
+  <si>
+    <t>Pesquet's Parrot</t>
+  </si>
+  <si>
+    <t>Psittrichas fulgidus</t>
+  </si>
+  <si>
+    <t>Pheasant Coucal</t>
+  </si>
+  <si>
+    <t>Centropus phasianinus</t>
+  </si>
+  <si>
+    <t>Pink-Eared Duck</t>
+  </si>
+  <si>
+    <t>Malacorhynchus membranaceus</t>
+  </si>
+  <si>
+    <t>Plains-Wanderer</t>
+  </si>
+  <si>
+    <t>Pedionomus torquatus</t>
+  </si>
+  <si>
+    <t>Princess Stephanie's Astrapia</t>
+  </si>
+  <si>
+    <t>Astrapia stephaniae</t>
+  </si>
+  <si>
+    <t>Pūkeko</t>
+  </si>
+  <si>
+    <t>Porphyrio melanotus</t>
+  </si>
+  <si>
+    <t>Rainbow Lorikeet</t>
+  </si>
+  <si>
+    <t>Trichoglossus moluccanus</t>
+  </si>
+  <si>
+    <t>Red Wattlebird</t>
+  </si>
+  <si>
+    <t>Anthochaera carunculata</t>
+  </si>
+  <si>
+    <t>Red-Backed Fairywren</t>
+  </si>
+  <si>
+    <t>Malurus melanocephalus</t>
+  </si>
+  <si>
+    <t>Red-Capped Robin</t>
+  </si>
+  <si>
+    <t>Petroica goodenovii</t>
+  </si>
+  <si>
+    <t>Red-Necked Avocet</t>
+  </si>
+  <si>
+    <t>Recurvirostra novaehollandiae</t>
+  </si>
+  <si>
+    <t>Red-Winged Parrot</t>
+  </si>
+  <si>
+    <t>Aprosmictus erythropterus</t>
+  </si>
+  <si>
+    <t>Regent Bowerbird</t>
+  </si>
+  <si>
+    <t>Sericulus chrysocephalus</t>
+  </si>
+  <si>
+    <t>Royal Spoonbill</t>
+  </si>
+  <si>
+    <t>Platalea regia</t>
+  </si>
+  <si>
+    <t>Rufous Night-Heron</t>
+  </si>
+  <si>
+    <t>Nycticorax caledonicus</t>
+  </si>
+  <si>
+    <t>Rufous Owl</t>
+  </si>
+  <si>
+    <t>Ninox rufa</t>
+  </si>
+  <si>
+    <t>Rufous-Banded Honeyeater</t>
+  </si>
+  <si>
+    <t>Conopophila albogularis</t>
+  </si>
+  <si>
+    <t>Sacred Kingfisher</t>
+  </si>
+  <si>
+    <t>Todiramphus sanctus</t>
+  </si>
+  <si>
+    <t>Silvereye</t>
+  </si>
+  <si>
+    <t>Zosterops lateralis</t>
+  </si>
+  <si>
+    <t>South Island Robin</t>
+  </si>
+  <si>
+    <t>Petroica australis</t>
+  </si>
+  <si>
+    <t>Southern Cassowary</t>
+  </si>
+  <si>
+    <t>Casuarius casuarius</t>
+  </si>
+  <si>
+    <t>Spangled Drongo</t>
+  </si>
+  <si>
+    <t>Dicrurus bracteatus</t>
+  </si>
+  <si>
+    <t>Splendid Fairywren</t>
+  </si>
+  <si>
+    <t>Malurus splendens</t>
+  </si>
+  <si>
+    <t>Spotless Crake</t>
+  </si>
+  <si>
+    <t>Zapornia tabuensis</t>
+  </si>
+  <si>
+    <t>Stubble Quail</t>
+  </si>
+  <si>
+    <t>Coturnix pectoralis</t>
+  </si>
+  <si>
+    <t>Sulphur-Crested Cockatoo</t>
+  </si>
+  <si>
+    <t>Cacatua galerita</t>
+  </si>
+  <si>
+    <t>Superb Lyrebird</t>
+  </si>
+  <si>
+    <t>Menura novaehollandiae</t>
+  </si>
+  <si>
+    <t>Tawny Frogmouth</t>
+  </si>
+  <si>
+    <t>Podargus strigoides</t>
+  </si>
+  <si>
+    <t>Tūī</t>
+  </si>
+  <si>
+    <t>Prosthemadera novaeseelandiae</t>
+  </si>
+  <si>
+    <t>Wedge-Tailed Eagle</t>
+  </si>
+  <si>
+    <t>Aquila audax</t>
+  </si>
+  <si>
+    <t>Welcome Swallow</t>
+  </si>
+  <si>
+    <t>Hirundo neoxena</t>
+  </si>
+  <si>
+    <t>White-Bellied Sea-Eagle</t>
+  </si>
+  <si>
+    <t>Haliaeetus leucogaster</t>
+  </si>
+  <si>
+    <t>White-Breasted Woodswallow</t>
+  </si>
+  <si>
+    <t>Artamus leucoryn</t>
+  </si>
+  <si>
+    <t>White-Faced Heron</t>
+  </si>
+  <si>
+    <t>Egretta novaehollandiae</t>
+  </si>
+  <si>
+    <t>Willie-Wagtail</t>
+  </si>
+  <si>
+    <t>Rhipidura leucophrys</t>
+  </si>
+  <si>
+    <t>Wrybill</t>
+  </si>
+  <si>
+    <t>Anarhynchus frontalis</t>
+  </si>
+  <si>
+    <t>Forest Data Analyst</t>
+  </si>
+  <si>
+    <t>Grassland Data Analyst</t>
+  </si>
+  <si>
+    <t>Mechanical Engineer</t>
+  </si>
+  <si>
+    <t>Site Selection Expert</t>
+  </si>
+  <si>
+    <t>Wetland Data Analyst</t>
   </si>
 </sst>
 </file>
@@ -2581,7 +3166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -2662,8 +3247,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24256CD6-671B-49BB-A76A-BCA812A8DD0C}" name="birds" displayName="birds" ref="A1:F262" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F262" xr:uid="{A51C43BE-DDEC-40D6-92FD-3C4BA38F764F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24256CD6-671B-49BB-A76A-BCA812A8DD0C}" name="birds" displayName="birds" ref="A1:F357" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F357" xr:uid="{A51C43BE-DDEC-40D6-92FD-3C4BA38F764F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{25ED0C0D-B939-406D-8B67-A9F9A8641DEE}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{72C3DFD8-3F0B-483B-8A68-A0BCCABA3E13}" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="10"/>
@@ -2677,8 +3262,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6299CC7B-9130-4C9A-A587-FBEBFEEB5D0F}" name="bonuses" displayName="bonuses" ref="A1:G34" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G34" xr:uid="{35D50B44-8490-4501-A753-CAF3081EA540}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6299CC7B-9130-4C9A-A587-FBEBFEEB5D0F}" name="bonuses" displayName="bonuses" ref="A1:G39" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G39" xr:uid="{35D50B44-8490-4501-A753-CAF3081EA540}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{339841CB-3C69-4C68-9375-1B8F78B4B947}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{7CD88691-F9EE-4A08-8F51-475C5497AC67}" uniqueName="2" name="English name" queryTableFieldId="2" dataDxfId="5"/>
@@ -2966,23 +3551,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F262"/>
+  <dimension ref="A1:F357"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D262"/>
+    <sheetView topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="A263" sqref="A263:C357"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3002,7 +3587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3022,7 +3607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3042,7 +3627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3062,7 +3647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3082,7 +3667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3102,7 +3687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3122,7 +3707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3142,7 +3727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3162,7 +3747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3182,7 +3767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3202,7 +3787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3222,7 +3807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3242,7 +3827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3262,7 +3847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3282,7 +3867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3302,7 +3887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3322,7 +3907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3342,7 +3927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3362,7 +3947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3382,7 +3967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3402,7 +3987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -3422,7 +4007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -3442,7 +4027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -3462,7 +4047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3482,7 +4067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -3502,7 +4087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -3522,7 +4107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -3542,7 +4127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -3562,7 +4147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>30</v>
       </c>
@@ -3582,7 +4167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3602,7 +4187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3622,7 +4207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3642,7 +4227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3662,7 +4247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3682,7 +4267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3702,7 +4287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3722,7 +4307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3742,7 +4327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -3762,7 +4347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3782,7 +4367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>41</v>
       </c>
@@ -3802,7 +4387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>42</v>
       </c>
@@ -3822,7 +4407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>43</v>
       </c>
@@ -3842,7 +4427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>44</v>
       </c>
@@ -3862,7 +4447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>45</v>
       </c>
@@ -3882,7 +4467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>46</v>
       </c>
@@ -3902,7 +4487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>47</v>
       </c>
@@ -3922,7 +4507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>48</v>
       </c>
@@ -3942,7 +4527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>49</v>
       </c>
@@ -3962,7 +4547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50</v>
       </c>
@@ -3982,7 +4567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>51</v>
       </c>
@@ -4002,7 +4587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>52</v>
       </c>
@@ -4022,7 +4607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>53</v>
       </c>
@@ -4042,7 +4627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>54</v>
       </c>
@@ -4062,7 +4647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>55</v>
       </c>
@@ -4082,7 +4667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>56</v>
       </c>
@@ -4102,7 +4687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>57</v>
       </c>
@@ -4122,7 +4707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>58</v>
       </c>
@@ -4142,7 +4727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>59</v>
       </c>
@@ -4162,7 +4747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>60</v>
       </c>
@@ -4182,7 +4767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>61</v>
       </c>
@@ -4202,7 +4787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>62</v>
       </c>
@@ -4222,7 +4807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>63</v>
       </c>
@@ -4242,7 +4827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>64</v>
       </c>
@@ -4262,7 +4847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>65</v>
       </c>
@@ -4282,7 +4867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>66</v>
       </c>
@@ -4302,7 +4887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>67</v>
       </c>
@@ -4322,7 +4907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>68</v>
       </c>
@@ -4342,7 +4927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>69</v>
       </c>
@@ -4362,7 +4947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>70</v>
       </c>
@@ -4382,7 +4967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4402,7 +4987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4422,7 +5007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4442,7 +5027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4462,7 +5047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4482,7 +5067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4502,7 +5087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4522,7 +5107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>78</v>
       </c>
@@ -4542,7 +5127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4562,7 +5147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4582,7 +5167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4602,7 +5187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4622,7 +5207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4642,7 +5227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4662,7 +5247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4682,7 +5267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4702,7 +5287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>87</v>
       </c>
@@ -4722,7 +5307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>88</v>
       </c>
@@ -4742,7 +5327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>89</v>
       </c>
@@ -4762,7 +5347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>90</v>
       </c>
@@ -4782,7 +5367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>91</v>
       </c>
@@ -4802,7 +5387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>92</v>
       </c>
@@ -4822,7 +5407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>93</v>
       </c>
@@ -4842,7 +5427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>94</v>
       </c>
@@ -4862,7 +5447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>95</v>
       </c>
@@ -4882,7 +5467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>96</v>
       </c>
@@ -4902,7 +5487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>97</v>
       </c>
@@ -4922,7 +5507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4942,7 +5527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4962,7 +5547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4982,7 +5567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>101</v>
       </c>
@@ -5002,7 +5587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>102</v>
       </c>
@@ -5022,7 +5607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>103</v>
       </c>
@@ -5042,7 +5627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>104</v>
       </c>
@@ -5062,7 +5647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>105</v>
       </c>
@@ -5082,7 +5667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>106</v>
       </c>
@@ -5102,7 +5687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>107</v>
       </c>
@@ -5122,7 +5707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>108</v>
       </c>
@@ -5142,7 +5727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>109</v>
       </c>
@@ -5162,7 +5747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>110</v>
       </c>
@@ -5182,7 +5767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>111</v>
       </c>
@@ -5202,7 +5787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>112</v>
       </c>
@@ -5222,7 +5807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>113</v>
       </c>
@@ -5242,7 +5827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>114</v>
       </c>
@@ -5262,7 +5847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>115</v>
       </c>
@@ -5282,7 +5867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5302,7 +5887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>117</v>
       </c>
@@ -5322,7 +5907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>118</v>
       </c>
@@ -5342,7 +5927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>119</v>
       </c>
@@ -5362,7 +5947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>120</v>
       </c>
@@ -5382,7 +5967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>121</v>
       </c>
@@ -5402,7 +5987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>122</v>
       </c>
@@ -5422,7 +6007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>123</v>
       </c>
@@ -5442,7 +6027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>124</v>
       </c>
@@ -5462,7 +6047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>125</v>
       </c>
@@ -5482,7 +6067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>126</v>
       </c>
@@ -5502,7 +6087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>127</v>
       </c>
@@ -5522,7 +6107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>128</v>
       </c>
@@ -5542,7 +6127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>129</v>
       </c>
@@ -5562,7 +6147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>130</v>
       </c>
@@ -5582,7 +6167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>131</v>
       </c>
@@ -5602,7 +6187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>132</v>
       </c>
@@ -5622,7 +6207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>133</v>
       </c>
@@ -5642,7 +6227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>134</v>
       </c>
@@ -5662,7 +6247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>135</v>
       </c>
@@ -5682,7 +6267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>136</v>
       </c>
@@ -5702,7 +6287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>137</v>
       </c>
@@ -5722,7 +6307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>138</v>
       </c>
@@ -5742,7 +6327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>139</v>
       </c>
@@ -5762,7 +6347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>140</v>
       </c>
@@ -5782,7 +6367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>141</v>
       </c>
@@ -5802,7 +6387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>142</v>
       </c>
@@ -5822,7 +6407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>143</v>
       </c>
@@ -5842,7 +6427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>144</v>
       </c>
@@ -5862,7 +6447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>145</v>
       </c>
@@ -5882,7 +6467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>146</v>
       </c>
@@ -5902,7 +6487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>147</v>
       </c>
@@ -5922,7 +6507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>148</v>
       </c>
@@ -5942,7 +6527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>149</v>
       </c>
@@ -5962,7 +6547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>150</v>
       </c>
@@ -5982,7 +6567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>151</v>
       </c>
@@ -6002,7 +6587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>152</v>
       </c>
@@ -6022,7 +6607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>153</v>
       </c>
@@ -6042,7 +6627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>154</v>
       </c>
@@ -6062,7 +6647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>155</v>
       </c>
@@ -6082,7 +6667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>156</v>
       </c>
@@ -6102,7 +6687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>157</v>
       </c>
@@ -6122,7 +6707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>158</v>
       </c>
@@ -6142,7 +6727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>159</v>
       </c>
@@ -6162,7 +6747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>160</v>
       </c>
@@ -6182,7 +6767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>161</v>
       </c>
@@ -6202,7 +6787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>162</v>
       </c>
@@ -6222,7 +6807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>163</v>
       </c>
@@ -6242,7 +6827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>164</v>
       </c>
@@ -6262,7 +6847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>165</v>
       </c>
@@ -6282,7 +6867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>166</v>
       </c>
@@ -6302,7 +6887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>167</v>
       </c>
@@ -6322,7 +6907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>168</v>
       </c>
@@ -6342,7 +6927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>169</v>
       </c>
@@ -6362,7 +6947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>170</v>
       </c>
@@ -6382,7 +6967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>171</v>
       </c>
@@ -6402,7 +6987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>172</v>
       </c>
@@ -6422,7 +7007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>173</v>
       </c>
@@ -6442,7 +7027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>174</v>
       </c>
@@ -6462,7 +7047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>175</v>
       </c>
@@ -6482,7 +7067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>176</v>
       </c>
@@ -6502,7 +7087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>177</v>
       </c>
@@ -6522,7 +7107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>178</v>
       </c>
@@ -6542,7 +7127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>179</v>
       </c>
@@ -6562,7 +7147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>180</v>
       </c>
@@ -6582,7 +7167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>181</v>
       </c>
@@ -6602,7 +7187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>182</v>
       </c>
@@ -6622,7 +7207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>183</v>
       </c>
@@ -6642,7 +7227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>184</v>
       </c>
@@ -6662,7 +7247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>185</v>
       </c>
@@ -6682,7 +7267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>186</v>
       </c>
@@ -6702,7 +7287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>187</v>
       </c>
@@ -6722,7 +7307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>188</v>
       </c>
@@ -6742,7 +7327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>189</v>
       </c>
@@ -6762,7 +7347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>190</v>
       </c>
@@ -6782,7 +7367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>191</v>
       </c>
@@ -6802,7 +7387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>192</v>
       </c>
@@ -6822,7 +7407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>193</v>
       </c>
@@ -6842,7 +7427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>194</v>
       </c>
@@ -6862,7 +7447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>195</v>
       </c>
@@ -6882,7 +7467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>196</v>
       </c>
@@ -6902,7 +7487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>197</v>
       </c>
@@ -6922,7 +7507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>198</v>
       </c>
@@ -6942,7 +7527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>199</v>
       </c>
@@ -6962,7 +7547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>200</v>
       </c>
@@ -6982,7 +7567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>201</v>
       </c>
@@ -7002,7 +7587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>203</v>
       </c>
@@ -7022,7 +7607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>204</v>
       </c>
@@ -7042,7 +7627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>205</v>
       </c>
@@ -7062,7 +7647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>206</v>
       </c>
@@ -7082,7 +7667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>207</v>
       </c>
@@ -7102,7 +7687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>208</v>
       </c>
@@ -7122,7 +7707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>209</v>
       </c>
@@ -7142,7 +7727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>210</v>
       </c>
@@ -7162,7 +7747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>211</v>
       </c>
@@ -7182,7 +7767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>212</v>
       </c>
@@ -7202,7 +7787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>213</v>
       </c>
@@ -7222,7 +7807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>214</v>
       </c>
@@ -7242,7 +7827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>215</v>
       </c>
@@ -7262,7 +7847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>216</v>
       </c>
@@ -7282,7 +7867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>217</v>
       </c>
@@ -7302,7 +7887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>218</v>
       </c>
@@ -7322,7 +7907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>219</v>
       </c>
@@ -7342,7 +7927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>220</v>
       </c>
@@ -7362,7 +7947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>221</v>
       </c>
@@ -7382,7 +7967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>222</v>
       </c>
@@ -7402,7 +7987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>223</v>
       </c>
@@ -7422,7 +8007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>224</v>
       </c>
@@ -7442,7 +8027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>225</v>
       </c>
@@ -7462,7 +8047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>226</v>
       </c>
@@ -7482,7 +8067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>227</v>
       </c>
@@ -7502,7 +8087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>228</v>
       </c>
@@ -7522,7 +8107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>229</v>
       </c>
@@ -7542,7 +8127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>230</v>
       </c>
@@ -7562,7 +8147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>231</v>
       </c>
@@ -7582,7 +8167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>232</v>
       </c>
@@ -7602,7 +8187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>233</v>
       </c>
@@ -7622,7 +8207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>234</v>
       </c>
@@ -7642,7 +8227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>235</v>
       </c>
@@ -7662,7 +8247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>236</v>
       </c>
@@ -7682,7 +8267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>237</v>
       </c>
@@ -7702,7 +8287,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>238</v>
       </c>
@@ -7722,7 +8307,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>239</v>
       </c>
@@ -7742,7 +8327,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>240</v>
       </c>
@@ -7762,7 +8347,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>241</v>
       </c>
@@ -7782,7 +8367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>242</v>
       </c>
@@ -7802,7 +8387,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>243</v>
       </c>
@@ -7822,7 +8407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>244</v>
       </c>
@@ -7842,7 +8427,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>245</v>
       </c>
@@ -7862,7 +8447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>246</v>
       </c>
@@ -7882,7 +8467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>247</v>
       </c>
@@ -7902,7 +8487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>248</v>
       </c>
@@ -7922,7 +8507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>249</v>
       </c>
@@ -7942,7 +8527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>250</v>
       </c>
@@ -7962,7 +8547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>251</v>
       </c>
@@ -7982,7 +8567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>252</v>
       </c>
@@ -8002,7 +8587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>253</v>
       </c>
@@ -8022,7 +8607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>254</v>
       </c>
@@ -8042,7 +8627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>255</v>
       </c>
@@ -8062,7 +8647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>256</v>
       </c>
@@ -8082,7 +8667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>257</v>
       </c>
@@ -8102,7 +8687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>258</v>
       </c>
@@ -8122,7 +8707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>259</v>
       </c>
@@ -8142,7 +8727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>260</v>
       </c>
@@ -8162,7 +8747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>261</v>
       </c>
@@ -8182,7 +8767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>262</v>
       </c>
@@ -8202,7 +8787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>263</v>
       </c>
@@ -8221,6 +8806,1336 @@
       <c r="F262" s="1" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>264</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="D263" s="1"/>
+      <c r="E263" s="1"/>
+      <c r="F263" s="1"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>265</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D264" s="1"/>
+      <c r="E264" s="1"/>
+      <c r="F264" s="1"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>266</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D265" s="1"/>
+      <c r="E265" s="1"/>
+      <c r="F265" s="1"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>267</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="D266" s="1"/>
+      <c r="E266" s="1"/>
+      <c r="F266" s="1"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>268</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="D267" s="1"/>
+      <c r="E267" s="1"/>
+      <c r="F267" s="1"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>269</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="D268" s="1"/>
+      <c r="E268" s="1"/>
+      <c r="F268" s="1"/>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>270</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D269" s="1"/>
+      <c r="E269" s="1"/>
+      <c r="F269" s="1"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>271</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D270" s="1"/>
+      <c r="E270" s="1"/>
+      <c r="F270" s="1"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>272</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D271" s="1"/>
+      <c r="E271" s="1"/>
+      <c r="F271" s="1"/>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>273</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D272" s="1"/>
+      <c r="E272" s="1"/>
+      <c r="F272" s="1"/>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>274</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="D273" s="1"/>
+      <c r="E273" s="1"/>
+      <c r="F273" s="1"/>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>275</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D274" s="1"/>
+      <c r="E274" s="1"/>
+      <c r="F274" s="1"/>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>276</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D275" s="1"/>
+      <c r="E275" s="1"/>
+      <c r="F275" s="1"/>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>277</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="D276" s="1"/>
+      <c r="E276" s="1"/>
+      <c r="F276" s="1"/>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>278</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="D277" s="1"/>
+      <c r="E277" s="1"/>
+      <c r="F277" s="1"/>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>279</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="D278" s="1"/>
+      <c r="E278" s="1"/>
+      <c r="F278" s="1"/>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>280</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="D279" s="1"/>
+      <c r="E279" s="1"/>
+      <c r="F279" s="1"/>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>281</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D280" s="1"/>
+      <c r="E280" s="1"/>
+      <c r="F280" s="1"/>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>282</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D281" s="1"/>
+      <c r="E281" s="1"/>
+      <c r="F281" s="1"/>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>283</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D282" s="1"/>
+      <c r="E282" s="1"/>
+      <c r="F282" s="1"/>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>284</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="D283" s="1"/>
+      <c r="E283" s="1"/>
+      <c r="F283" s="1"/>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>285</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D284" s="1"/>
+      <c r="E284" s="1"/>
+      <c r="F284" s="1"/>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>286</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="D285" s="1"/>
+      <c r="E285" s="1"/>
+      <c r="F285" s="1"/>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>287</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="D286" s="1"/>
+      <c r="E286" s="1"/>
+      <c r="F286" s="1"/>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>288</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="D287" s="1"/>
+      <c r="E287" s="1"/>
+      <c r="F287" s="1"/>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>289</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D288" s="1"/>
+      <c r="E288" s="1"/>
+      <c r="F288" s="1"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>290</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D289" s="1"/>
+      <c r="E289" s="1"/>
+      <c r="F289" s="1"/>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>291</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D290" s="1"/>
+      <c r="E290" s="1"/>
+      <c r="F290" s="1"/>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>292</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="D291" s="1"/>
+      <c r="E291" s="1"/>
+      <c r="F291" s="1"/>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>293</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="D292" s="1"/>
+      <c r="E292" s="1"/>
+      <c r="F292" s="1"/>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>294</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="D293" s="1"/>
+      <c r="E293" s="1"/>
+      <c r="F293" s="1"/>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>295</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D294" s="1"/>
+      <c r="E294" s="1"/>
+      <c r="F294" s="1"/>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>296</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D295" s="1"/>
+      <c r="E295" s="1"/>
+      <c r="F295" s="1"/>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>297</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="D296" s="1"/>
+      <c r="E296" s="1"/>
+      <c r="F296" s="1"/>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>298</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D297" s="1"/>
+      <c r="E297" s="1"/>
+      <c r="F297" s="1"/>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>299</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D298" s="1"/>
+      <c r="E298" s="1"/>
+      <c r="F298" s="1"/>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>300</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D299" s="1"/>
+      <c r="E299" s="1"/>
+      <c r="F299" s="1"/>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>301</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="D300" s="1"/>
+      <c r="E300" s="1"/>
+      <c r="F300" s="1"/>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>302</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D301" s="1"/>
+      <c r="E301" s="1"/>
+      <c r="F301" s="1"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>303</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="D302" s="1"/>
+      <c r="E302" s="1"/>
+      <c r="F302" s="1"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>304</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D303" s="1"/>
+      <c r="E303" s="1"/>
+      <c r="F303" s="1"/>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>305</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D304" s="1"/>
+      <c r="E304" s="1"/>
+      <c r="F304" s="1"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>306</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D305" s="1"/>
+      <c r="E305" s="1"/>
+      <c r="F305" s="1"/>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>307</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D306" s="1"/>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1"/>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>308</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="D307" s="1"/>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1"/>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>309</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="D308" s="1"/>
+      <c r="E308" s="1"/>
+      <c r="F308" s="1"/>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>310</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="D309" s="1"/>
+      <c r="E309" s="1"/>
+      <c r="F309" s="1"/>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>311</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D310" s="1"/>
+      <c r="E310" s="1"/>
+      <c r="F310" s="1"/>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>312</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D311" s="1"/>
+      <c r="E311" s="1"/>
+      <c r="F311" s="1"/>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>313</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="D312" s="1"/>
+      <c r="E312" s="1"/>
+      <c r="F312" s="1"/>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>314</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="D313" s="1"/>
+      <c r="E313" s="1"/>
+      <c r="F313" s="1"/>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>315</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="D314" s="1"/>
+      <c r="E314" s="1"/>
+      <c r="F314" s="1"/>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>316</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="D315" s="1"/>
+      <c r="E315" s="1"/>
+      <c r="F315" s="1"/>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>317</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D316" s="1"/>
+      <c r="E316" s="1"/>
+      <c r="F316" s="1"/>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>318</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="D317" s="1"/>
+      <c r="E317" s="1"/>
+      <c r="F317" s="1"/>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>319</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="D318" s="1"/>
+      <c r="E318" s="1"/>
+      <c r="F318" s="1"/>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>320</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="D319" s="1"/>
+      <c r="E319" s="1"/>
+      <c r="F319" s="1"/>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>321</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="D320" s="1"/>
+      <c r="E320" s="1"/>
+      <c r="F320" s="1"/>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>322</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="D321" s="1"/>
+      <c r="E321" s="1"/>
+      <c r="F321" s="1"/>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>323</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="D322" s="1"/>
+      <c r="E322" s="1"/>
+      <c r="F322" s="1"/>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>324</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D323" s="1"/>
+      <c r="E323" s="1"/>
+      <c r="F323" s="1"/>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>325</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="D324" s="1"/>
+      <c r="E324" s="1"/>
+      <c r="F324" s="1"/>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>326</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="D325" s="1"/>
+      <c r="E325" s="1"/>
+      <c r="F325" s="1"/>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>327</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="D326" s="1"/>
+      <c r="E326" s="1"/>
+      <c r="F326" s="1"/>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>328</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D327" s="1"/>
+      <c r="E327" s="1"/>
+      <c r="F327" s="1"/>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>329</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="D328" s="1"/>
+      <c r="E328" s="1"/>
+      <c r="F328" s="1"/>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>330</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="C329" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D329" s="1"/>
+      <c r="E329" s="1"/>
+      <c r="F329" s="1"/>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>331</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="D330" s="1"/>
+      <c r="E330" s="1"/>
+      <c r="F330" s="1"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>332</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D331" s="1"/>
+      <c r="E331" s="1"/>
+      <c r="F331" s="1"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>333</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="D332" s="1"/>
+      <c r="E332" s="1"/>
+      <c r="F332" s="1"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>334</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="D333" s="1"/>
+      <c r="E333" s="1"/>
+      <c r="F333" s="1"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>335</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D334" s="1"/>
+      <c r="E334" s="1"/>
+      <c r="F334" s="1"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>336</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D335" s="1"/>
+      <c r="E335" s="1"/>
+      <c r="F335" s="1"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>337</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D336" s="1"/>
+      <c r="E336" s="1"/>
+      <c r="F336" s="1"/>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>338</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="D337" s="1"/>
+      <c r="E337" s="1"/>
+      <c r="F337" s="1"/>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>339</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="D338" s="1"/>
+      <c r="E338" s="1"/>
+      <c r="F338" s="1"/>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>340</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="D339" s="1"/>
+      <c r="E339" s="1"/>
+      <c r="F339" s="1"/>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>341</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="D340" s="1"/>
+      <c r="E340" s="1"/>
+      <c r="F340" s="1"/>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>342</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D341" s="1"/>
+      <c r="E341" s="1"/>
+      <c r="F341" s="1"/>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>343</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D342" s="1"/>
+      <c r="E342" s="1"/>
+      <c r="F342" s="1"/>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>344</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D343" s="1"/>
+      <c r="E343" s="1"/>
+      <c r="F343" s="1"/>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>345</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D344" s="1"/>
+      <c r="E344" s="1"/>
+      <c r="F344" s="1"/>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>346</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D345" s="1"/>
+      <c r="E345" s="1"/>
+      <c r="F345" s="1"/>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>347</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D346" s="1"/>
+      <c r="E346" s="1"/>
+      <c r="F346" s="1"/>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>348</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D347" s="1"/>
+      <c r="E347" s="1"/>
+      <c r="F347" s="1"/>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>349</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D348" s="1"/>
+      <c r="E348" s="1"/>
+      <c r="F348" s="1"/>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>350</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D349" s="1"/>
+      <c r="E349" s="1"/>
+      <c r="F349" s="1"/>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>351</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D350" s="1"/>
+      <c r="E350" s="1"/>
+      <c r="F350" s="1"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>352</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D351" s="1"/>
+      <c r="E351" s="1"/>
+      <c r="F351" s="1"/>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>353</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D352" s="1"/>
+      <c r="E352" s="1"/>
+      <c r="F352" s="1"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A353">
+        <v>354</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D353" s="1"/>
+      <c r="E353" s="1"/>
+      <c r="F353" s="1"/>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A354">
+        <v>355</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D354" s="1"/>
+      <c r="E354" s="1"/>
+      <c r="F354" s="1"/>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A355">
+        <v>356</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C355" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D355" s="1"/>
+      <c r="E355" s="1"/>
+      <c r="F355" s="1"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A356">
+        <v>357</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D356" s="1"/>
+      <c r="E356" s="1"/>
+      <c r="F356" s="1"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A357">
+        <v>358</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D357" s="1"/>
+      <c r="E357" s="1"/>
+      <c r="F357" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8232,22 +10147,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F73C7-BAF7-4DDB-A3F3-74A889132A9F}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8270,7 +10187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8293,7 +10210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -8316,7 +10233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -8339,7 +10256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -8362,7 +10279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -8385,7 +10302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -8408,7 +10325,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -8431,7 +10348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -8454,7 +10371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -8477,7 +10394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -8500,7 +10417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -8523,7 +10440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -8546,7 +10463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -8569,7 +10486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -8592,7 +10509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -8615,7 +10532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -8638,7 +10555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -8661,7 +10578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -8684,7 +10601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -8707,7 +10624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -8730,7 +10647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -8753,7 +10670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1021</v>
       </c>
@@ -8776,7 +10693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1022</v>
       </c>
@@ -8799,7 +10716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1023</v>
       </c>
@@ -8822,7 +10739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1024</v>
       </c>
@@ -8845,7 +10762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1025</v>
       </c>
@@ -8868,7 +10785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1026</v>
       </c>
@@ -8891,7 +10808,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1027</v>
       </c>
@@ -8914,7 +10831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1028</v>
       </c>
@@ -8937,7 +10854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1029</v>
       </c>
@@ -8960,7 +10877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1030</v>
       </c>
@@ -8983,7 +10900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1031</v>
       </c>
@@ -9006,7 +10923,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1032</v>
       </c>
@@ -9028,6 +10945,71 @@
       <c r="G34" s="1" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1033</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1034</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1035</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1036</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1037</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9045,13 +11027,13 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.9296875" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9059,27 +11041,27 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>571</v>
       </c>

</xml_diff>

<commit_message>
Add yellow power field to translation tables
</commit_message>
<xml_diff>
--- a/i18n/de.xlsx
+++ b/i18n/de.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matej\Programming\wingsearch\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AA659A-B4F0-45E8-9ED2-A42034AA28FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B1A993-BC3A-459E-B25E-FC76FAEF22FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="1028">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="1029">
   <si>
     <t>id</t>
   </si>
@@ -3126,16 +3126,25 @@
   </si>
   <si>
     <t>Wetland Data Analyst</t>
+  </si>
+  <si>
+    <t>GAME END</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3278,8 +3287,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AA05F43-7971-4EB4-8E5C-9E7EFB591048}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{A5CFAA4D-6579-4D29-89EB-6C57AE6E1FEB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AA05F43-7971-4EB4-8E5C-9E7EFB591048}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{A5CFAA4D-6579-4D29-89EB-6C57AE6E1FEB}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{EA688C91-7F6D-4D7A-9D79-A30EB35759F6}" name="English name"/>
     <tableColumn id="2" xr3:uid="{3A0CACDB-DCE4-4775-8258-271B6485FC6A}" name="Translated"/>
@@ -10149,7 +10158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F73C7-BAF7-4DDB-A3F3-74A889132A9F}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:B39"/>
     </sheetView>
   </sheetViews>
@@ -11021,10 +11030,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D758ED0-344A-47B5-8000-C5BBB7F38038}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11063,10 +11072,16 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>571</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
fix cards match (#43)
</commit_message>
<xml_diff>
--- a/i18n/de.xlsx
+++ b/i18n/de.xlsx
@@ -3668,9 +3668,9 @@
   <dimension ref="A1:J357"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E163" activeCellId="0" sqref="E163"/>
+      <selection pane="bottomLeft" activeCell="A201" activeCellId="0" sqref="A201:A357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8197,7 +8197,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>662</v>
@@ -8221,7 +8221,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>665</v>
@@ -8245,7 +8245,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="n">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>668</v>
@@ -8271,7 +8271,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="n">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>672</v>
@@ -8295,7 +8295,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="n">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>675</v>
@@ -8319,7 +8319,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="n">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>678</v>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="n">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>681</v>
@@ -8365,7 +8365,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="n">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>684</v>
@@ -8389,7 +8389,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="n">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>687</v>
@@ -8413,7 +8413,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>690</v>
@@ -8437,7 +8437,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>693</v>
@@ -8461,7 +8461,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>696</v>
@@ -8483,7 +8483,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>699</v>
@@ -8505,7 +8505,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="n">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>703</v>
@@ -8527,7 +8527,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="n">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>706</v>
@@ -8551,7 +8551,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="n">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>709</v>
@@ -8575,7 +8575,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>713</v>
@@ -8595,7 +8595,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="n">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>716</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="n">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>719</v>
@@ -8637,7 +8637,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="n">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>722</v>
@@ -8661,7 +8661,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="n">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>726</v>
@@ -8683,7 +8683,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="n">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>730</v>
@@ -8705,7 +8705,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="n">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>733</v>
@@ -8729,7 +8729,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>736</v>
@@ -8749,7 +8749,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="n">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>739</v>
@@ -8769,7 +8769,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="n">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>742</v>
@@ -8789,7 +8789,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="n">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>745</v>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B229" s="2" t="s">
         <v>748</v>
@@ -8831,7 +8831,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B230" s="2" t="s">
         <v>751</v>
@@ -8855,7 +8855,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="n">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B231" s="2" t="s">
         <v>755</v>
@@ -8875,7 +8875,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B232" s="2" t="s">
         <v>758</v>
@@ -8895,7 +8895,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="n">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B233" s="2" t="s">
         <v>761</v>
@@ -8917,7 +8917,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="n">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B234" s="2" t="s">
         <v>765</v>
@@ -8937,7 +8937,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="n">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B235" s="2" t="s">
         <v>768</v>
@@ -8957,7 +8957,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="n">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B236" s="2" t="s">
         <v>771</v>
@@ -8977,7 +8977,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="n">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B237" s="2" t="s">
         <v>774</v>
@@ -8999,7 +8999,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="n">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B238" s="2" t="s">
         <v>777</v>
@@ -9019,7 +9019,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="n">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B239" s="2" t="s">
         <v>780</v>
@@ -9041,7 +9041,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="n">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B240" s="2" t="s">
         <v>783</v>
@@ -9063,7 +9063,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="n">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B241" s="2" t="s">
         <v>786</v>
@@ -9085,7 +9085,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="n">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B242" s="2" t="s">
         <v>789</v>
@@ -9109,7 +9109,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="n">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B243" s="2" t="s">
         <v>792</v>
@@ -9135,7 +9135,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="n">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B244" s="2" t="s">
         <v>795</v>
@@ -9161,7 +9161,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="n">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>799</v>
@@ -9185,7 +9185,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>802</v>
@@ -9209,7 +9209,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="n">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>805</v>
@@ -9233,7 +9233,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="n">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>808</v>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="n">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B249" s="2" t="s">
         <v>811</v>
@@ -9283,7 +9283,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="n">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B250" s="2" t="s">
         <v>814</v>
@@ -9303,7 +9303,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="n">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>817</v>
@@ -9323,7 +9323,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="n">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>820</v>
@@ -9343,7 +9343,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="n">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>823</v>
@@ -9365,7 +9365,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="n">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B254" s="2" t="s">
         <v>826</v>
@@ -9387,7 +9387,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="n">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B255" s="2" t="s">
         <v>829</v>
@@ -9407,7 +9407,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="n">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B256" s="2" t="s">
         <v>832</v>
@@ -9427,7 +9427,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="n">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>835</v>
@@ -9451,7 +9451,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>838</v>
@@ -9475,7 +9475,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="n">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>841</v>
@@ -9499,7 +9499,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="n">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B260" s="2" t="s">
         <v>844</v>
@@ -9523,7 +9523,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="n">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B261" s="2" t="s">
         <v>847</v>
@@ -9547,7 +9547,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="n">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B262" s="2" t="s">
         <v>850</v>
@@ -9571,7 +9571,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="n">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>853</v>
@@ -9591,7 +9591,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="n">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>855</v>
@@ -9611,7 +9611,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="n">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>857</v>
@@ -9631,7 +9631,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="n">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>859</v>
@@ -9651,7 +9651,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="n">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>861</v>
@@ -9671,7 +9671,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="n">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>863</v>
@@ -9691,7 +9691,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="n">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>865</v>
@@ -9711,7 +9711,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="n">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>867</v>
@@ -9731,7 +9731,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="n">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>869</v>
@@ -9751,7 +9751,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="n">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B272" s="2" t="s">
         <v>871</v>
@@ -9771,7 +9771,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="n">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B273" s="2" t="s">
         <v>873</v>
@@ -9791,7 +9791,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="n">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B274" s="2" t="s">
         <v>875</v>
@@ -9811,7 +9811,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B275" s="2" t="s">
         <v>877</v>
@@ -9833,7 +9833,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="n">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>879</v>
@@ -9853,7 +9853,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="n">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B277" s="2" t="s">
         <v>881</v>
@@ -9871,7 +9871,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="n">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B278" s="2" t="s">
         <v>883</v>
@@ -9891,7 +9891,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="n">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>885</v>
@@ -9909,7 +9909,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B280" s="2" t="s">
         <v>887</v>
@@ -9927,7 +9927,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="n">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B281" s="2" t="s">
         <v>889</v>
@@ -9947,7 +9947,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="n">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B282" s="2" t="s">
         <v>891</v>
@@ -9967,7 +9967,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="n">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B283" s="2" t="s">
         <v>893</v>
@@ -9987,7 +9987,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="n">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B284" s="2" t="s">
         <v>895</v>
@@ -10009,7 +10009,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="n">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B285" s="2" t="s">
         <v>897</v>
@@ -10029,7 +10029,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="n">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B286" s="2" t="s">
         <v>899</v>
@@ -10047,7 +10047,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="n">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B287" s="2" t="s">
         <v>901</v>
@@ -10065,7 +10065,7 @@
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="n">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B288" s="2" t="s">
         <v>903</v>
@@ -10087,7 +10087,7 @@
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="n">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B289" s="2" t="s">
         <v>905</v>
@@ -10107,7 +10107,7 @@
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="n">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>907</v>
@@ -10127,7 +10127,7 @@
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="n">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>909</v>
@@ -10147,7 +10147,7 @@
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="n">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B292" s="2" t="s">
         <v>911</v>
@@ -10167,7 +10167,7 @@
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="n">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B293" s="2" t="s">
         <v>913</v>
@@ -10187,7 +10187,7 @@
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="n">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B294" s="2" t="s">
         <v>915</v>
@@ -10207,7 +10207,7 @@
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="n">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B295" s="2" t="s">
         <v>917</v>
@@ -10229,7 +10229,7 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="n">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B296" s="2" t="s">
         <v>919</v>
@@ -10251,7 +10251,7 @@
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="n">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B297" s="2" t="s">
         <v>921</v>
@@ -10271,7 +10271,7 @@
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="n">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B298" s="2" t="s">
         <v>923</v>
@@ -10289,7 +10289,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="n">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B299" s="2" t="s">
         <v>925</v>
@@ -10307,7 +10307,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="n">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B300" s="2" t="s">
         <v>927</v>
@@ -10325,7 +10325,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B301" s="2" t="s">
         <v>929</v>
@@ -10343,7 +10343,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="n">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B302" s="2" t="s">
         <v>931</v>
@@ -10361,7 +10361,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="n">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B303" s="2" t="s">
         <v>933</v>
@@ -10379,7 +10379,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="n">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B304" s="2" t="s">
         <v>935</v>
@@ -10397,7 +10397,7 @@
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="n">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B305" s="2" t="s">
         <v>937</v>
@@ -10417,7 +10417,7 @@
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="1" t="n">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B306" s="2" t="s">
         <v>939</v>
@@ -10435,7 +10435,7 @@
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="1" t="n">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B307" s="2" t="s">
         <v>941</v>
@@ -10453,7 +10453,7 @@
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="1" t="n">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B308" s="2" t="s">
         <v>943</v>
@@ -10471,7 +10471,7 @@
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="1" t="n">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B309" s="2" t="s">
         <v>945</v>
@@ -10491,7 +10491,7 @@
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="1" t="n">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B310" s="2" t="s">
         <v>947</v>
@@ -10511,7 +10511,7 @@
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="1" t="n">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B311" s="2" t="s">
         <v>949</v>
@@ -10529,7 +10529,7 @@
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="1" t="n">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B312" s="2" t="s">
         <v>951</v>
@@ -10547,7 +10547,7 @@
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="1" t="n">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>953</v>
@@ -10567,7 +10567,7 @@
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="1" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>955</v>
@@ -10585,7 +10585,7 @@
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="1" t="n">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>957</v>
@@ -10603,7 +10603,7 @@
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="1" t="n">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B316" s="2" t="s">
         <v>959</v>
@@ -10623,7 +10623,7 @@
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="1" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>961</v>
@@ -10641,7 +10641,7 @@
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="1" t="n">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>963</v>
@@ -10663,7 +10663,7 @@
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="1" t="n">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>965</v>
@@ -10687,7 +10687,7 @@
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="n">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>967</v>
@@ -10709,7 +10709,7 @@
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="1" t="n">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>969</v>
@@ -10727,7 +10727,7 @@
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="1" t="n">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>971</v>
@@ -10747,7 +10747,7 @@
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="1" t="n">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>973</v>
@@ -10765,7 +10765,7 @@
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="1" t="n">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>975</v>
@@ -10787,7 +10787,7 @@
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="n">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>977</v>
@@ -10809,7 +10809,7 @@
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="1" t="n">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>979</v>
@@ -10827,7 +10827,7 @@
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="1" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>981</v>
@@ -10845,7 +10845,7 @@
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="n">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>983</v>
@@ -10863,7 +10863,7 @@
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="1" t="n">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>985</v>
@@ -10885,7 +10885,7 @@
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="1" t="n">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>987</v>
@@ -10907,7 +10907,7 @@
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="1" t="n">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>989</v>
@@ -10929,7 +10929,7 @@
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="1" t="n">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>991</v>
@@ -10951,7 +10951,7 @@
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="1" t="n">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>993</v>
@@ -10973,7 +10973,7 @@
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="1" t="n">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B334" s="2" t="s">
         <v>995</v>
@@ -10991,7 +10991,7 @@
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="1" t="n">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B335" s="2" t="s">
         <v>997</v>
@@ -11011,7 +11011,7 @@
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="1" t="n">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B336" s="2" t="s">
         <v>999</v>
@@ -11031,7 +11031,7 @@
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="1" t="n">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B337" s="2" t="s">
         <v>1001</v>
@@ -11051,7 +11051,7 @@
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="1" t="n">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B338" s="2" t="s">
         <v>1003</v>
@@ -11071,7 +11071,7 @@
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="1" t="n">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B339" s="2" t="s">
         <v>1005</v>
@@ -11089,7 +11089,7 @@
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="1" t="n">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B340" s="2" t="s">
         <v>1007</v>
@@ -11111,7 +11111,7 @@
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="1" t="n">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B341" s="2" t="s">
         <v>1009</v>
@@ -11131,7 +11131,7 @@
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="1" t="n">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B342" s="2" t="s">
         <v>1011</v>
@@ -11151,7 +11151,7 @@
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="1" t="n">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B343" s="2" t="s">
         <v>1013</v>
@@ -11169,7 +11169,7 @@
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="1" t="n">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B344" s="2" t="s">
         <v>1015</v>
@@ -11187,7 +11187,7 @@
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="1" t="n">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B345" s="2" t="s">
         <v>1017</v>
@@ -11205,7 +11205,7 @@
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="1" t="n">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B346" s="2" t="s">
         <v>1019</v>
@@ -11223,7 +11223,7 @@
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="1" t="n">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B347" s="2" t="s">
         <v>1021</v>
@@ -11245,7 +11245,7 @@
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="n">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B348" s="2" t="s">
         <v>1023</v>
@@ -11265,7 +11265,7 @@
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="1" t="n">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B349" s="2" t="s">
         <v>1025</v>
@@ -11289,7 +11289,7 @@
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="1" t="n">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B350" s="2" t="s">
         <v>1027</v>
@@ -11307,7 +11307,7 @@
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="1" t="n">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B351" s="2" t="s">
         <v>1029</v>
@@ -11327,7 +11327,7 @@
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="1" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B352" s="2" t="s">
         <v>1031</v>
@@ -11345,7 +11345,7 @@
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="1" t="n">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B353" s="2" t="s">
         <v>1033</v>
@@ -11369,7 +11369,7 @@
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="1" t="n">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B354" s="2" t="s">
         <v>1035</v>
@@ -11391,7 +11391,7 @@
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="1" t="n">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B355" s="2" t="s">
         <v>1037</v>
@@ -11413,7 +11413,7 @@
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="1" t="n">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B356" s="2" t="s">
         <v>1039</v>
@@ -11435,7 +11435,7 @@
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="1" t="n">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B357" s="2" t="s">
         <v>1041</v>
@@ -11475,7 +11475,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="1" sqref="A201:A357 G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12087,7 +12087,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A201:A357 B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
parameters: show bonus icons
</commit_message>
<xml_diff>
--- a/i18n/de.xlsx
+++ b/i18n/de.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$447</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ExternalData_2" vbProcedure="false">Bonuses!$A$1:$H$60</definedName>
   </definedNames>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="1785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1787">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -5440,19 +5442,19 @@
     <t xml:space="preserve">Bei Aktivierung </t>
   </si>
   <si>
-    <t xml:space="preserve">WHEN PLAYED</t>
+    <t xml:space="preserve">WHEN PLAYED</t>
   </si>
   <si>
     <t xml:space="preserve">Beim Ausspeieln </t>
   </si>
   <si>
-    <t xml:space="preserve">ONCE BETWEEN TURNS</t>
+    <t xml:space="preserve">ONCE BETWEEN TURNS</t>
   </si>
   <si>
     <t xml:space="preserve">1x zwischen deinen Zügen </t>
   </si>
   <si>
-    <t xml:space="preserve">ROUND END</t>
+    <t xml:space="preserve">ROUND END</t>
   </si>
   <si>
     <t xml:space="preserve">Am Rundenende </t>
@@ -5464,19 +5466,28 @@
     <t xml:space="preserve">Am Spielende</t>
   </si>
   <si>
-    <t xml:space="preserve">of cards</t>
+    <t xml:space="preserve">of cards</t>
   </si>
   <si>
     <t xml:space="preserve">der Karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show bonus cards match symbols</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$SFr.-807]\ #,##0.00;[RED][$SFr.-807]&quot; -&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
+    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -5611,7 +5622,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5652,6 +5663,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5682,6 +5709,10 @@
     </dxf>
   </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16235,7 +16266,7 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
@@ -17407,7 +17438,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17425,8 +17456,8 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1773</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -17434,7 +17465,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1775</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -17442,31 +17473,31 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>1777</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1778</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>1779</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1780</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>1781</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1782</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>1783</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -17485,4 +17516,51 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B2" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B2"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Show language-dependent bonus icons systematically (#78)
* parameters: show bonus icons

* Fix wrong 'parameters' type declarations and refactor

* Publish changes
</commit_message>
<xml_diff>
--- a/i18n/de.xlsx
+++ b/i18n/de.xlsx
@@ -5,14 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$B$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$447</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="ExternalData_2" vbProcedure="false">Bonuses!$A$1:$H$60</definedName>
   </definedNames>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="1785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="1787">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -5440,19 +5442,19 @@
     <t xml:space="preserve">Bei Aktivierung </t>
   </si>
   <si>
-    <t xml:space="preserve">WHEN PLAYED</t>
+    <t xml:space="preserve">WHEN PLAYED</t>
   </si>
   <si>
     <t xml:space="preserve">Beim Ausspeieln </t>
   </si>
   <si>
-    <t xml:space="preserve">ONCE BETWEEN TURNS</t>
+    <t xml:space="preserve">ONCE BETWEEN TURNS</t>
   </si>
   <si>
     <t xml:space="preserve">1x zwischen deinen Zügen </t>
   </si>
   <si>
-    <t xml:space="preserve">ROUND END</t>
+    <t xml:space="preserve">ROUND END</t>
   </si>
   <si>
     <t xml:space="preserve">Am Rundenende </t>
@@ -5464,19 +5466,28 @@
     <t xml:space="preserve">Am Spielende</t>
   </si>
   <si>
-    <t xml:space="preserve">of cards</t>
+    <t xml:space="preserve">of cards</t>
   </si>
   <si>
     <t xml:space="preserve">der Karten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show bonus cards match symbols</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$SFr.-807]\ #,##0.00;[RED][$SFr.-807]&quot; -&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
+    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -5611,7 +5622,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5652,6 +5663,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5682,6 +5709,10 @@
     </dxf>
   </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16235,7 +16266,7 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
@@ -17407,7 +17438,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17425,8 +17456,8 @@
         <v>1772</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1773</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -17434,7 +17465,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1775</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -17442,31 +17473,31 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>1777</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1778</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>1779</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>1780</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>1781</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1782</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>1783</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -17485,4 +17516,51 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.95"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B2" s="13" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B2"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normalny"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normalny"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>